<commit_message>
Nescafe Test Case added
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/Nobel_Yayin_TC1.xlsx
+++ b/src/test/java/apachePOI/Nobel_Yayin_TC1.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -357,6 +357,36 @@
   </si>
   <si>
     <t>vrwqmea8@gmail.com</t>
+  </si>
+  <si>
+    <t>660r1cw6@gmail.com</t>
+  </si>
+  <si>
+    <t>a9ausm0a@yahoo.com</t>
+  </si>
+  <si>
+    <t>sfna3ug2@yahoo.com</t>
+  </si>
+  <si>
+    <t>68zoqph9@yahoo.com</t>
+  </si>
+  <si>
+    <t>vgt9znho@gmail.com</t>
+  </si>
+  <si>
+    <t>re7guys3@hotmail.com</t>
+  </si>
+  <si>
+    <t>egptfjaz@hotmail.com</t>
+  </si>
+  <si>
+    <t>46qhzob0@example.com</t>
+  </si>
+  <si>
+    <t>oicmm8g9@gmail.com</t>
+  </si>
+  <si>
+    <t>04p9ig59@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -757,7 +787,7 @@
         <v>5462345687</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>2</v>
@@ -777,7 +807,7 @@
         <v>5462345687</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>2</v>
@@ -797,7 +827,7 @@
         <v>5462345687</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>2</v>
@@ -817,7 +847,7 @@
         <v>5462345687</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>2</v>
@@ -837,7 +867,7 @@
         <v>5462345687</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>2</v>
@@ -857,7 +887,7 @@
         <v>5462345687</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>2</v>
@@ -877,7 +907,7 @@
         <v>5462345687</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>2</v>
@@ -897,7 +927,7 @@
         <v>5462345687</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>2</v>
@@ -917,7 +947,7 @@
         <v>5462345687</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F10" t="s" s="0">
         <v>2</v>
@@ -937,7 +967,7 @@
         <v>5462345687</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>2</v>

</xml_diff>